<commit_message>
Updated data on excel file
</commit_message>
<xml_diff>
--- a/2018-2012_FIES_excel_data.xlsx
+++ b/2018-2012_FIES_excel_data.xlsx
@@ -874,7 +874,7 @@
         <v>211000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="29.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -924,7 +924,7 @@
         <v>243000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="29.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -974,7 +974,7 @@
         <v>138000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="29.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>144000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="29.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>163000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="29.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>164000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="29.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>132000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="29.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>122000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="29.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>143000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="29.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>156000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="29.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1374,12 +1374,12 @@
         <v>140000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="29.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2">
-        <v>1225</v>
+        <v>657143</v>
       </c>
       <c r="C18" s="2">
         <v>105870437507</v>

</xml_diff>